<commit_message>
Query de la base de datos finalizado
</commit_message>
<xml_diff>
--- a/Proyecto Ferreteira - 1/DataBase/NormalizacionBDferreteria.xlsx
+++ b/Proyecto Ferreteira - 1/DataBase/NormalizacionBDferreteria.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d958853a2a55a1f/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge Ayala\Proyecto-ferreteria\Proyecto Ferreteira - 1\DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{FD1252FC-F388-4CAD-BE86-52C0F11B14A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2F585EE9-0625-439C-B64E-16C39E7F7269}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926A7641-261A-4091-A599-E16E79AB7061}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10E161DC-B631-4D8E-8534-C87E98A98220}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="67">
   <si>
     <t>codigo_venta</t>
   </si>
@@ -211,9 +211,6 @@
   </si>
   <si>
     <t>Precio_estandar</t>
-  </si>
-  <si>
-    <t>codigo_repartidor</t>
   </si>
   <si>
     <t>Esquemas</t>
@@ -637,7 +634,7 @@
   <dimension ref="B3:J64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,7 +957,7 @@
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D38" t="s">
         <v>1</v>
@@ -977,7 +974,7 @@
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>8</v>
@@ -994,7 +991,7 @@
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>44</v>
@@ -1011,7 +1008,7 @@
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D41" t="s">
         <v>24</v>
@@ -1022,7 +1019,7 @@
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D42" t="s">
         <v>9</v>
@@ -1076,7 +1073,7 @@
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F48" t="s">
@@ -1133,7 +1130,7 @@
     </row>
     <row r="52" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D52" s="4" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="F52" t="s">
         <v>46</v>

</xml_diff>